<commit_message>
Adicionando dados de professores dos arquivos de Annabell
</commit_message>
<xml_diff>
--- a/Files/data/Relação Professor x Disciplina.xlsx
+++ b/Files/data/Relação Professor x Disciplina.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HDExt\GitHub\9Semestre\timetabling-UENF\Files\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9C61B8-0C7B-4E13-9518-18F6AEBB8128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734E1D16-72F0-4138-98A3-99C8DC1D7DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F98ED11F-55C7-446D-8B4A-1C78A975CED3}"/>
   </bookViews>
@@ -882,8 +882,8 @@
   <dimension ref="A1:V64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I6:I7"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,11 +962,11 @@
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
+      <c r="A2" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -987,10 +987,10 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1002,10 +1002,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1014,7 +1014,7 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -1030,11 +1030,11 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>51</v>
+      <c r="A3" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1055,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -1098,11 +1098,11 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
+      <c r="A4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1123,13 +1123,13 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -1166,11 +1166,11 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
+      <c r="A5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1191,10 +1191,10 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1234,50 +1234,50 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
+      <c r="A6" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1302,50 +1302,50 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>138</v>
+      <c r="A7" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1370,32 +1370,32 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>53</v>
+      <c r="A8" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1407,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1439,10 +1439,10 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1463,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1506,29 +1506,29 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>143</v>
+      <c r="A10" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1574,29 +1574,29 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>144</v>
+      <c r="A11" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>142</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -1642,29 +1642,29 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>71</v>
+      <c r="A12" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1691,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -1710,29 +1710,29 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
+      <c r="A13" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1741,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1778,29 +1778,29 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>85</v>
+      <c r="A14" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1836,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -1846,29 +1846,29 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>109</v>
+      <c r="A15" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>0</v>
@@ -1914,29 +1914,29 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>75</v>
+      <c r="A16" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -1982,29 +1982,29 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
+      <c r="A17" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -2050,29 +2050,29 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>37</v>
+      <c r="A18" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2114,33 +2114,33 @@
         <v>0</v>
       </c>
       <c r="V18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>61</v>
+      <c r="A19" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>112</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2182,33 +2182,33 @@
         <v>0</v>
       </c>
       <c r="V19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>39</v>
+      <c r="A20" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2250,33 +2250,33 @@
         <v>0</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>65</v>
+      <c r="A21" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -2318,33 +2318,33 @@
         <v>0</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>55</v>
+      <c r="A22" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2386,33 +2386,33 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>47</v>
+      <c r="A23" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -2451,36 +2451,36 @@
         <v>0</v>
       </c>
       <c r="U23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V23">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>25</v>
+      <c r="A24" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -2519,36 +2519,36 @@
         <v>0</v>
       </c>
       <c r="U24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V24">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>43</v>
+      <c r="A25" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2590,33 +2590,33 @@
         <v>0</v>
       </c>
       <c r="V25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>89</v>
+      <c r="A26" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2658,15 +2658,15 @@
         <v>0</v>
       </c>
       <c r="V26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2731,10 +2731,10 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2799,10 +2799,10 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2867,10 +2867,10 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2935,10 +2935,10 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2959,7 +2959,7 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -2980,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="P31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -3003,10 +3003,10 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -3275,10 +3275,10 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -3343,10 +3343,10 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -3411,10 +3411,10 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -3479,10 +3479,10 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -3547,10 +3547,10 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3614,29 +3614,29 @@
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>77</v>
+      <c r="A41" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -3678,33 +3678,33 @@
         <v>0</v>
       </c>
       <c r="V41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>101</v>
+      <c r="A42" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -3746,33 +3746,33 @@
         <v>0</v>
       </c>
       <c r="V42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>117</v>
+      <c r="A43" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>26</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -3811,36 +3811,36 @@
         <v>0</v>
       </c>
       <c r="U43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V43">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>113</v>
+      <c r="A44" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -3879,36 +3879,36 @@
         <v>0</v>
       </c>
       <c r="U44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V44">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>115</v>
+      <c r="A45" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -3950,33 +3950,33 @@
         <v>0</v>
       </c>
       <c r="V45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>103</v>
+      <c r="A46" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -4018,33 +4018,33 @@
         <v>0</v>
       </c>
       <c r="V46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>111</v>
+      <c r="A47" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -4086,33 +4086,33 @@
         <v>0</v>
       </c>
       <c r="V47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>93</v>
+      <c r="A48" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -4154,33 +4154,33 @@
         <v>0</v>
       </c>
       <c r="V48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>107</v>
+      <c r="A49" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>38</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -4222,42 +4222,42 @@
         <v>0</v>
       </c>
       <c r="V49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>73</v>
+      <c r="A50" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -4294,29 +4294,29 @@
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>79</v>
+      <c r="A51" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51">
         <v>0</v>
@@ -4362,35 +4362,35 @@
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>83</v>
+      <c r="A52" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -4430,35 +4430,35 @@
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>81</v>
+      <c r="A53" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -4470,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -4498,29 +4498,29 @@
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>35</v>
+      <c r="A54" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54">
         <v>0</v>
@@ -4544,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="P54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54">
         <v>0</v>
@@ -4566,29 +4566,29 @@
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>29</v>
+      <c r="A55" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -4597,7 +4597,7 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -4634,29 +4634,29 @@
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>41</v>
+      <c r="A56" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -4668,7 +4668,7 @@
         <v>0</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56">
         <v>0</v>
@@ -4683,7 +4683,7 @@
         <v>0</v>
       </c>
       <c r="Q56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R56">
         <v>0</v>
@@ -4702,35 +4702,35 @@
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>9</v>
+      <c r="A57" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -4742,10 +4742,10 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P57">
         <v>0</v>
@@ -4770,50 +4770,50 @@
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>3</v>
+      <c r="A58" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58">
         <v>0</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58">
         <v>0</v>
       </c>
       <c r="M58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N58">
         <v>0</v>
       </c>
       <c r="O58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P58">
         <v>0</v>
@@ -4838,32 +4838,32 @@
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>27</v>
+      <c r="A59" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B59" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -4875,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -4906,50 +4906,50 @@
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>5</v>
+      <c r="A60" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60">
         <v>0</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60">
         <v>0</v>
       </c>
       <c r="M60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N60">
         <v>0</v>
       </c>
       <c r="O60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P60">
         <v>0</v>
@@ -4974,11 +4974,11 @@
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>19</v>
+      <c r="A61" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -5014,7 +5014,7 @@
         <v>0</v>
       </c>
       <c r="N61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -5026,7 +5026,7 @@
         <v>0</v>
       </c>
       <c r="R61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61">
         <v>0</v>
@@ -5042,11 +5042,11 @@
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>13</v>
+      <c r="A62" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -5082,7 +5082,7 @@
         <v>0</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O62">
         <v>0</v>
@@ -5094,7 +5094,7 @@
         <v>0</v>
       </c>
       <c r="R62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S62">
         <v>0</v>
@@ -5110,11 +5110,11 @@
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>57</v>
+      <c r="A63" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -5162,10 +5162,10 @@
         <v>0</v>
       </c>
       <c r="R63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T63">
         <v>0</v>
@@ -5178,11 +5178,11 @@
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>33</v>
+      <c r="A64" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -5230,13 +5230,13 @@
         <v>0</v>
       </c>
       <c r="R64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S64">
         <v>0</v>
       </c>
       <c r="T64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U64">
         <v>0</v>
@@ -5248,7 +5248,7 @@
   </sheetData>
   <autoFilter ref="A1:V1" xr:uid="{6794BEBD-A37D-4817-8711-7D2B9E60B04B}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V64">
-      <sortCondition descending="1" ref="J1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C2:V64">

</xml_diff>